<commit_message>
Edits to leave out whitening process
</commit_message>
<xml_diff>
--- a/progress/8_26_13/baseline_9_subjects_adjusted.xlsx
+++ b/progress/8_26_13/baseline_9_subjects_adjusted.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10720" yWindow="-80" windowWidth="21600" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="10520" yWindow="-80" windowWidth="21600" windowHeight="15320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1 vs 2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="39">
   <si>
     <t>Subject A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -159,6 +159,22 @@
   </si>
   <si>
     <t>Variance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with lnorm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with lnorm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w/o whiten</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w/0 whiten</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -166,6 +182,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -538,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView view="pageLayout" topLeftCell="F64" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -585,6 +607,9 @@
       <c r="D3">
         <v>83.33</v>
       </c>
+      <c r="E3">
+        <v>71.67</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -599,6 +624,9 @@
       <c r="D4">
         <v>81.67</v>
       </c>
+      <c r="E4">
+        <v>76.67</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -613,6 +641,9 @@
       <c r="D5">
         <v>81.67</v>
       </c>
+      <c r="E5">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
@@ -627,6 +658,9 @@
       <c r="D6">
         <v>81.67</v>
       </c>
+      <c r="E6">
+        <v>75</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
@@ -641,6 +675,9 @@
       <c r="D7">
         <v>88.33</v>
       </c>
+      <c r="E7">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1">
       <c r="A9" s="2" t="s">
@@ -658,9 +695,9 @@
         <f t="shared" si="0"/>
         <v>83.334000000000003</v>
       </c>
-      <c r="E9" s="2" t="e">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>74.668000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -700,6 +737,9 @@
       <c r="D14">
         <v>76.67</v>
       </c>
+      <c r="E14">
+        <v>71.67</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
@@ -714,6 +754,9 @@
       <c r="D15">
         <v>71.67</v>
       </c>
+      <c r="E15">
+        <v>71.67</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
@@ -728,6 +771,9 @@
       <c r="D16">
         <v>80</v>
       </c>
+      <c r="E16">
+        <v>75</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
@@ -742,6 +788,9 @@
       <c r="D17">
         <v>76.67</v>
       </c>
+      <c r="E17">
+        <v>75</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
@@ -756,6 +805,9 @@
       <c r="D18">
         <v>75</v>
       </c>
+      <c r="E18">
+        <v>73.33</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
@@ -773,9 +825,9 @@
         <f t="shared" si="1"/>
         <v>76.001999999999995</v>
       </c>
-      <c r="E20" s="2" t="e">
+      <c r="E20" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>73.334000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -810,6 +862,9 @@
       <c r="D25">
         <v>70</v>
       </c>
+      <c r="E25">
+        <v>61.67</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
@@ -824,6 +879,9 @@
       <c r="D26">
         <v>71.67</v>
       </c>
+      <c r="E26">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
@@ -838,6 +896,9 @@
       <c r="D27">
         <v>60</v>
       </c>
+      <c r="E27">
+        <v>63.33</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
@@ -852,6 +913,9 @@
       <c r="D28">
         <v>68.33</v>
       </c>
+      <c r="E28">
+        <v>71.67</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
@@ -866,6 +930,9 @@
       <c r="D29">
         <v>60</v>
       </c>
+      <c r="E29">
+        <v>58.33</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
@@ -883,17 +950,17 @@
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="E31" s="2" t="e">
+      <c r="E31" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:6">
       <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
@@ -906,8 +973,11 @@
       <c r="E35" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -920,8 +990,14 @@
       <c r="D36">
         <v>75</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="E36">
+        <v>78.33</v>
+      </c>
+      <c r="F36">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -934,8 +1010,14 @@
       <c r="D37">
         <v>81.67</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="E37">
+        <v>85</v>
+      </c>
+      <c r="F37">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -948,8 +1030,14 @@
       <c r="D38">
         <v>85</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="E38">
+        <v>88.33</v>
+      </c>
+      <c r="F38">
+        <v>86.67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -962,8 +1050,14 @@
       <c r="D39">
         <v>88.33</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="E39">
+        <v>86.67</v>
+      </c>
+      <c r="F39">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -976,13 +1070,19 @@
       <c r="D40">
         <v>78.33</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="E40">
+        <v>73.33</v>
+      </c>
+      <c r="F40">
+        <v>78.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="2">
-        <f t="shared" ref="B42:E42" si="3">AVERAGE(B36:B40)</f>
+        <f t="shared" ref="B42:F42" si="3">AVERAGE(B36:B40)</f>
         <v>88.33</v>
       </c>
       <c r="C42" s="2">
@@ -993,9 +1093,13 @@
         <f t="shared" si="3"/>
         <v>81.665999999999997</v>
       </c>
-      <c r="E42" s="2" t="e">
+      <c r="E42" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>82.331999999999994</v>
+      </c>
+      <c r="F42" s="2">
+        <f t="shared" si="3"/>
+        <v>79.994</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1030,6 +1134,9 @@
       <c r="D52">
         <v>71.67</v>
       </c>
+      <c r="E52">
+        <v>71.67</v>
+      </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
@@ -1044,6 +1151,9 @@
       <c r="D53">
         <v>75</v>
       </c>
+      <c r="E53">
+        <v>80</v>
+      </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
@@ -1058,6 +1168,9 @@
       <c r="D54">
         <v>70</v>
       </c>
+      <c r="E54">
+        <v>73.33</v>
+      </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
@@ -1072,6 +1185,9 @@
       <c r="D55">
         <v>73.33</v>
       </c>
+      <c r="E55">
+        <v>76.67</v>
+      </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
@@ -1086,6 +1202,9 @@
       <c r="D56">
         <v>75</v>
       </c>
+      <c r="E56">
+        <v>78.33</v>
+      </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
@@ -1103,9 +1222,9 @@
         <f t="shared" si="4"/>
         <v>73</v>
       </c>
-      <c r="E58" s="2" t="e">
+      <c r="E58" s="2">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1140,6 +1259,9 @@
       <c r="D63">
         <v>66.67</v>
       </c>
+      <c r="E63">
+        <v>70</v>
+      </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
@@ -1154,6 +1276,9 @@
       <c r="D64">
         <v>63.33</v>
       </c>
+      <c r="E64">
+        <v>73.33</v>
+      </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
@@ -1168,6 +1293,9 @@
       <c r="D65">
         <v>56.67</v>
       </c>
+      <c r="E65">
+        <v>75</v>
+      </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
@@ -1182,6 +1310,9 @@
       <c r="D66">
         <v>61.67</v>
       </c>
+      <c r="E66">
+        <v>76.67</v>
+      </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
@@ -1196,6 +1327,9 @@
       <c r="D67">
         <v>61.67</v>
       </c>
+      <c r="E67">
+        <v>71.67</v>
+      </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="2" t="s">
@@ -1213,9 +1347,9 @@
         <f t="shared" si="5"/>
         <v>62.00200000000001</v>
       </c>
-      <c r="E69" s="2" t="e">
+      <c r="E69" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>73.334000000000003</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1250,6 +1384,9 @@
       <c r="D74">
         <v>66.67</v>
       </c>
+      <c r="E74">
+        <v>70</v>
+      </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
@@ -1264,6 +1401,9 @@
       <c r="D75">
         <v>71.67</v>
       </c>
+      <c r="E75">
+        <v>73.33</v>
+      </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
@@ -1278,6 +1418,9 @@
       <c r="D76">
         <v>73.33</v>
       </c>
+      <c r="E76">
+        <v>75</v>
+      </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
@@ -1292,6 +1435,9 @@
       <c r="D77">
         <v>71.67</v>
       </c>
+      <c r="E77">
+        <v>76.67</v>
+      </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
@@ -1306,6 +1452,9 @@
       <c r="D78">
         <v>68.33</v>
       </c>
+      <c r="E78">
+        <v>71.67</v>
+      </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="2" t="s">
@@ -1323,17 +1472,17 @@
         <f t="shared" si="6"/>
         <v>70.334000000000003</v>
       </c>
-      <c r="E80" s="2" t="e">
+      <c r="E80" s="2">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+        <v>73.334000000000003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:8">
       <c r="B84" s="1" t="s">
         <v>1</v>
       </c>
@@ -1346,8 +1495,14 @@
       <c r="E84" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84" t="s">
+        <v>36</v>
+      </c>
+      <c r="G84" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>2</v>
       </c>
@@ -1360,8 +1515,20 @@
       <c r="D85">
         <v>73.33</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="E85">
+        <v>63.33</v>
+      </c>
+      <c r="F85">
+        <v>56.67</v>
+      </c>
+      <c r="G85">
+        <v>68.33</v>
+      </c>
+      <c r="H85">
+        <v>71.67</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>3</v>
       </c>
@@ -1374,8 +1541,20 @@
       <c r="D86">
         <v>66.67</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="E86">
+        <v>60</v>
+      </c>
+      <c r="F86">
+        <v>58.33</v>
+      </c>
+      <c r="G86">
+        <v>68.33</v>
+      </c>
+      <c r="H86">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -1388,8 +1567,20 @@
       <c r="D87">
         <v>61.67</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="E87">
+        <v>63.33</v>
+      </c>
+      <c r="F87">
+        <v>55</v>
+      </c>
+      <c r="G87">
+        <v>68.33</v>
+      </c>
+      <c r="H87">
+        <v>71.67</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -1402,8 +1593,20 @@
       <c r="D88">
         <v>51.67</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="E88">
+        <v>63.33</v>
+      </c>
+      <c r="F88">
+        <v>46.7</v>
+      </c>
+      <c r="G88">
+        <v>63.33</v>
+      </c>
+      <c r="H88">
+        <v>71.67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -1416,13 +1619,25 @@
       <c r="D89">
         <v>66.67</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="E89">
+        <v>50</v>
+      </c>
+      <c r="F89">
+        <v>51.6</v>
+      </c>
+      <c r="G89">
+        <v>70</v>
+      </c>
+      <c r="H89">
+        <v>73.33</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B91" s="2">
-        <f t="shared" ref="B91:E91" si="7">AVERAGE(B85:B89)</f>
+        <f t="shared" ref="B91:H91" si="7">AVERAGE(B85:B89)</f>
         <v>77.001999999999995</v>
       </c>
       <c r="C91" s="2">
@@ -1433,17 +1648,29 @@
         <f t="shared" si="7"/>
         <v>64.00200000000001</v>
       </c>
-      <c r="E91" s="2" t="e">
+      <c r="E91" s="2">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
+        <v>59.998000000000005</v>
+      </c>
+      <c r="F91" s="2">
+        <f t="shared" si="7"/>
+        <v>53.660000000000004</v>
+      </c>
+      <c r="G91" s="2">
+        <f t="shared" si="7"/>
+        <v>67.664000000000001</v>
+      </c>
+      <c r="H91" s="2">
+        <f t="shared" si="7"/>
+        <v>71.001999999999995</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:7">
       <c r="B100" s="1" t="s">
         <v>1</v>
       </c>
@@ -1457,7 +1684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>2</v>
       </c>
@@ -1471,7 +1698,7 @@
         <v>48.33</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
         <v>3</v>
       </c>
@@ -1485,7 +1712,7 @@
         <v>61.67</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:7">
       <c r="A103" t="s">
         <v>4</v>
       </c>
@@ -1499,7 +1726,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:7">
       <c r="A104" t="s">
         <v>5</v>
       </c>
@@ -1513,7 +1740,7 @@
         <v>68.33</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:7">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -1527,12 +1754,12 @@
         <v>63.33</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:7">
       <c r="A107" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B107" s="2">
-        <f t="shared" ref="B107:E107" si="8">AVERAGE(B101:B105)</f>
+        <f t="shared" ref="B107:G107" si="8">AVERAGE(B101:B105)</f>
         <v>83.665999999999997</v>
       </c>
       <c r="C107" s="2">
@@ -1544,6 +1771,14 @@
         <v>59.331999999999994</v>
       </c>
       <c r="E107" s="2" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F107" s="2" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G107" s="2" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
@@ -1566,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1586,9 +1821,6 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
         <v>33</v>
       </c>
@@ -1859,26 +2091,26 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:6">
       <c r="B35" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
-      <c r="D35" t="s">
-        <v>9</v>
-      </c>
       <c r="E35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -1888,8 +2120,11 @@
       <c r="C36">
         <v>90</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <v>86.67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1899,8 +2134,11 @@
       <c r="C37">
         <v>93.33</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <v>86.67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1910,8 +2148,11 @@
       <c r="C38">
         <v>90</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38">
+        <v>96.67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1921,8 +2162,11 @@
       <c r="C39">
         <v>93.33</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <v>86.67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1932,8 +2176,11 @@
       <c r="C40">
         <v>93.33</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F40">
+        <v>93.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>7</v>
       </c>
@@ -1942,17 +2189,18 @@
         <v>96.665999999999997</v>
       </c>
       <c r="C42" s="2">
-        <f t="shared" ref="C42:E42" si="6">AVERAGE(C36:C40)</f>
+        <f t="shared" ref="C42:F42" si="6">AVERAGE(C36:C40)</f>
         <v>91.99799999999999</v>
       </c>
-      <c r="D42" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="D42" s="2"/>
       <c r="E42" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="F42" s="2">
+        <f t="shared" ref="F42" si="7">AVERAGE(F36:F40)</f>
+        <v>89.996000000000009</v>
+      </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
@@ -2033,19 +2281,19 @@
         <v>26</v>
       </c>
       <c r="B58" s="2">
-        <f t="shared" ref="B58" si="7">AVERAGE(B52:B56)</f>
+        <f t="shared" ref="B58" si="8">AVERAGE(B52:B56)</f>
         <v>91.331999999999994</v>
       </c>
       <c r="C58" s="2">
-        <f t="shared" ref="C58:E58" si="8">AVERAGE(C52:C56)</f>
+        <f t="shared" ref="C58:E58" si="9">AVERAGE(C52:C56)</f>
         <v>87.332000000000008</v>
       </c>
       <c r="D58" s="2" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E58" s="2" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2128,19 +2376,19 @@
         <v>7</v>
       </c>
       <c r="B69" s="2">
-        <f t="shared" ref="B69" si="9">AVERAGE(B63:B67)</f>
+        <f t="shared" ref="B69" si="10">AVERAGE(B63:B67)</f>
         <v>92</v>
       </c>
       <c r="C69" s="2">
-        <f t="shared" ref="C69:E69" si="10">AVERAGE(C63:C67)</f>
+        <f t="shared" ref="C69:E69" si="11">AVERAGE(C63:C67)</f>
         <v>67.331999999999994</v>
       </c>
       <c r="D69" s="2" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E69" s="2" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2223,28 +2471,28 @@
         <v>7</v>
       </c>
       <c r="B80" s="2">
-        <f t="shared" ref="B80" si="11">AVERAGE(B74:B78)</f>
+        <f t="shared" ref="B80" si="12">AVERAGE(B74:B78)</f>
         <v>88.665999999999997</v>
       </c>
       <c r="C80" s="2">
-        <f t="shared" ref="C80:E80" si="12">AVERAGE(C74:C78)</f>
+        <f t="shared" ref="C80:E80" si="13">AVERAGE(C74:C78)</f>
         <v>73.334000000000003</v>
       </c>
       <c r="D80" s="2" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E80" s="2" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:8">
       <c r="B84" s="1" t="s">
         <v>31</v>
       </c>
@@ -2257,8 +2505,11 @@
       <c r="E84" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="G84" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>2</v>
       </c>
@@ -2268,8 +2519,17 @@
       <c r="C85">
         <v>70</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85">
+        <v>53.33</v>
+      </c>
+      <c r="G85">
+        <v>73.33</v>
+      </c>
+      <c r="H85">
+        <v>76.67</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>3</v>
       </c>
@@ -2279,8 +2539,17 @@
       <c r="C86">
         <v>76.67</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86">
+        <v>66.67</v>
+      </c>
+      <c r="G86">
+        <v>80</v>
+      </c>
+      <c r="H86">
+        <v>73.33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -2290,8 +2559,17 @@
       <c r="C87">
         <v>73.33</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87">
+        <v>63.33</v>
+      </c>
+      <c r="G87">
+        <v>83.33</v>
+      </c>
+      <c r="H87">
+        <v>86.67</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -2301,8 +2579,17 @@
       <c r="C88">
         <v>60</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88">
+        <v>53.3</v>
+      </c>
+      <c r="G88">
+        <v>73.33</v>
+      </c>
+      <c r="H88">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -2312,26 +2599,47 @@
       <c r="C89">
         <v>76.67</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F89">
+        <v>50</v>
+      </c>
+      <c r="G89">
+        <v>86.67</v>
+      </c>
+      <c r="H89">
+        <v>86.67</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B91" s="2">
-        <f t="shared" ref="B91" si="13">AVERAGE(B85:B89)</f>
+        <f t="shared" ref="B91" si="14">AVERAGE(B85:B89)</f>
         <v>84.00200000000001</v>
       </c>
       <c r="C91" s="2">
-        <f t="shared" ref="C91:E91" si="14">AVERAGE(C85:C89)</f>
+        <f t="shared" ref="C91:H91" si="15">AVERAGE(C85:C89)</f>
         <v>71.334000000000003</v>
       </c>
       <c r="D91" s="2" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E91" s="2" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="F91" s="2">
+        <f t="shared" si="15"/>
+        <v>57.326000000000001</v>
+      </c>
+      <c r="G91" s="2">
+        <f t="shared" si="15"/>
+        <v>79.331999999999994</v>
+      </c>
+      <c r="H91" s="2">
+        <f t="shared" si="15"/>
+        <v>80.668000000000006</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2413,19 +2721,19 @@
         <v>7</v>
       </c>
       <c r="B107" s="2">
-        <f t="shared" ref="B107" si="15">AVERAGE(B101:B105)</f>
+        <f t="shared" ref="B107" si="16">AVERAGE(B101:B105)</f>
         <v>93.331999999999994</v>
       </c>
       <c r="C107" s="2">
-        <f t="shared" ref="C107:E107" si="16">AVERAGE(C101:C105)</f>
+        <f t="shared" ref="C107:E107" si="17">AVERAGE(C101:C105)</f>
         <v>72.665999999999997</v>
       </c>
       <c r="D107" s="2" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E107" s="2" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>